<commit_message>
changed chart area three year scatter
</commit_message>
<xml_diff>
--- a/data/projectStats.xlsx
+++ b/data/projectStats.xlsx
@@ -433,7 +433,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -483,7 +483,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2">

</xml_diff>